<commit_message>
[Add] Test Flow, Test Steps, Pom Classes & [Enhance] Custom Listener
</commit_message>
<xml_diff>
--- a/Data Files/Web_SauceDemo_Test_Data.xlsx
+++ b/Data Files/Web_SauceDemo_Test_Data.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12435"/>
+    <workbookView windowHeight="18285"/>
   </bookViews>
   <sheets>
-    <sheet name="ahromiSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Order" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>ScenarioId</t>
   </si>
@@ -38,19 +38,40 @@
     <t>Password</t>
   </si>
   <si>
-    <t>P_001_PositiveScenarios</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>adminPassword</t>
-  </si>
-  <si>
-    <t>P_002_NegativeScenarios</t>
-  </si>
-  <si>
-    <t>wrongPassword</t>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>P_001_Order_With_Multiple_Items</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>Backpack;Onesie;T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>Lukman</t>
+  </si>
+  <si>
+    <t>Ahromi</t>
+  </si>
+  <si>
+    <t>44556677</t>
+  </si>
+  <si>
+    <t>N_001_Checkout_With_Invalid_Payment</t>
   </si>
 </sst>
 </file>
@@ -63,7 +84,7 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +100,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -229,12 +258,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -438,17 +473,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,55 +605,52 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -633,82 +665,94 @@
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1243,20 +1287,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="24.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="9.71428571428571" customWidth="1"/>
+    <col min="1" max="1" width="40.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="15.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="30.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="10.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="11.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1266,28 +1313,56 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
+    <row r="2" spans="1:7">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>